<commit_message>
CHANGE Miilon - Add more vocabulary.
</commit_message>
<xml_diff>
--- a/MiilonData/EditoB2_unite2_p32.xlsx
+++ b/MiilonData/EditoB2_unite2_p32.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
   <si>
     <t>Grammaire</t>
   </si>
@@ -135,6 +135,93 @@
   </si>
   <si>
     <t>pískat, hvízdat, syčet, fičet, sípat</t>
+  </si>
+  <si>
+    <t>abeille</t>
+  </si>
+  <si>
+    <t>nf</t>
+  </si>
+  <si>
+    <t>abej</t>
+  </si>
+  <si>
+    <t>včela</t>
+  </si>
+  <si>
+    <t>chat</t>
+  </si>
+  <si>
+    <t>nm</t>
+  </si>
+  <si>
+    <t>ša</t>
+  </si>
+  <si>
+    <t>kočka, kocour</t>
+  </si>
+  <si>
+    <t>chien</t>
+  </si>
+  <si>
+    <t>šje~</t>
+  </si>
+  <si>
+    <t>pes</t>
+  </si>
+  <si>
+    <t>coq</t>
+  </si>
+  <si>
+    <t>kok</t>
+  </si>
+  <si>
+    <t>kohout</t>
+  </si>
+  <si>
+    <t>loup</t>
+  </si>
+  <si>
+    <t>lu</t>
+  </si>
+  <si>
+    <t>vlk</t>
+  </si>
+  <si>
+    <t>mouton</t>
+  </si>
+  <si>
+    <t>muto~</t>
+  </si>
+  <si>
+    <t>skopec, beránek</t>
+  </si>
+  <si>
+    <t>oiseau</t>
+  </si>
+  <si>
+    <t>u^azo.</t>
+  </si>
+  <si>
+    <t>pták</t>
+  </si>
+  <si>
+    <t>perroquet</t>
+  </si>
+  <si>
+    <t>peroke</t>
+  </si>
+  <si>
+    <t>papoušek</t>
+  </si>
+  <si>
+    <t>vache</t>
+  </si>
+  <si>
+    <t>vaš</t>
+  </si>
+  <si>
+    <t>kráva</t>
   </si>
 </sst>
 </file>
@@ -519,10 +606,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,6 +814,168 @@
         <v>{ "foreign": "siffler", "grammar": "vi", "pronunciation": "sifle.", "meaning": "pískat, hvízdat, syčet, fičet, sípat" },</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" ref="F13:F21" si="1" xml:space="preserve"> "{ ""foreign"": """ &amp; A13 &amp; """, ""grammar"": """ &amp; B13 &amp; """, ""pronunciation"": """ &amp; C13 &amp; """, ""meaning"": """ &amp; D13 &amp; """ },"</f>
+        <v>{ "foreign": "abeille", "grammar": "nf", "pronunciation": "abej", "meaning": "včela" },</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="1"/>
+        <v>{ "foreign": "chat", "grammar": "nm", "pronunciation": "ša", "meaning": "kočka, kocour" },</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="1"/>
+        <v>{ "foreign": "chien", "grammar": "nm", "pronunciation": "šje~", "meaning": "pes" },</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="1"/>
+        <v>{ "foreign": "coq", "grammar": "nm", "pronunciation": "kok", "meaning": "kohout" },</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="1"/>
+        <v>{ "foreign": "loup", "grammar": "nm", "pronunciation": "lu", "meaning": "vlk" },</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="1"/>
+        <v>{ "foreign": "mouton", "grammar": "nm", "pronunciation": "muto~", "meaning": "skopec, beránek" },</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="1"/>
+        <v>{ "foreign": "oiseau", "grammar": "nm", "pronunciation": "u^azo.", "meaning": "pták" },</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="1"/>
+        <v>{ "foreign": "perroquet", "grammar": "nm", "pronunciation": "peroke", "meaning": "papoušek" },</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="1"/>
+        <v>{ "foreign": "vache", "grammar": "nf", "pronunciation": "vaš", "meaning": "kráva" },</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>